<commit_message>
Regenerate tables and main figures from final dual-VIIRS dataset
</commit_message>
<xml_diff>
--- a/results/Tables.xlsx
+++ b/results/Tables.xlsx
@@ -440,32 +440,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>iso3</t>
+          <t>Country (ISO3)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>total_hansen_loss_Mha</t>
+          <t>Total Hansen loss 2015–2023 (Mha)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>mean_annual_loss_kha</t>
+          <t>Mean annual Hansen loss (kha)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>mean_discrepancy_ratio</t>
+          <t>Mean discrepancy ratio (Hansen/FRA)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>mean_protected_share</t>
+          <t>Mean protected-loss share</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>total_viirs_M</t>
+          <t>Total VIIRS fire detections (millions)</t>
         </is>
       </c>
     </row>
@@ -753,27 +753,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>iso3</t>
+          <t>Country (ISO3)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>hansen_loss_kha</t>
+          <t>Hansen loss (kha)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>fao_net_change_kha</t>
+          <t>FRA net forest area change (kha)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>discrepancy_ratio</t>
+          <t>Discrepancy ratio (Hansen/FRA)</t>
         </is>
       </c>
     </row>
@@ -1477,22 +1477,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>iso3</t>
+          <t>Country (ISO3)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>protected_loss_share_mean</t>
+          <t>Mean protected-loss share</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>protected_loss_share_max</t>
+          <t>Maximum protected-loss share</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>year_of_max</t>
+          <t>Year of maximum protected-loss share</t>
         </is>
       </c>
     </row>
@@ -1710,27 +1710,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>iso3</t>
+          <t>Country (ISO3)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pearson_corr</t>
+          <t>Pearson correlation (Hansen vs VIIRS)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>slope_ha_per_fire</t>
+          <t>Slope (ha per detection)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>intercept</t>
+          <t>Intercept (ha)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>p_value</t>
+          <t>p-value</t>
         </is>
       </c>
     </row>
@@ -1984,17 +1984,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>iso3</t>
+          <t>Country (ISO3)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>max_abs_diff_kha</t>
+          <t>Max absolute difference (kha)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>mean_abs_diff_kha</t>
+          <t>Mean absolute difference (kha)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean appendix table headings (no underscores)
</commit_message>
<xml_diff>
--- a/results/Tables.xlsx
+++ b/results/Tables.xlsx
@@ -12,6 +12,8 @@
     <sheet name="Table3_protected_share" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Table4_fire_loss_corr" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Table5_interp_check" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TableA1_discrepancy_ratios" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TableA2_fire_loss_corr_sorted" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2157,4 +2159,499 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country (ISO3)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ARG</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1.095996440146589</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8027770353969796</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.201690072363169</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BOL</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2.345918699311887</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.65258765793092</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.898758930285535</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BRA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2.260176146447278</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.9505106100654231</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8420619971346361</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CHL</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>47.9543009184719</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9.413422224394401</v>
+      </c>
+      <c r="D5" t="n">
+        <v>21.4823597782565</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.907426298753638</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.390356715730083</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.341511600125703</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ECU</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6264072316900283</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.464226115823015</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.224966079563679</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GUY</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.582132641486334</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.491279382962717</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3.556369363481102</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PER</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.128650839916678</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.341478153156763</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.7385605665069043</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PRY</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.111295844283485</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.307075365266392</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.102986604058451</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SUR</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.73008185564031</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.039166524348505</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.374601431569341</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>URY</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>VEN</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.51988724059989</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.107808190268713</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.17198458393493</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country (ISO3)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Pearson correlation (Hansen vs VIIRS)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Slope (ha per detection)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Intercept (ha)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GUY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.8064161669000441</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.418961741659722</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3310.845789785792</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.008647339703521884</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BOL</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7274446375198309</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.231106557890573</v>
+      </c>
+      <c r="D3" t="n">
+        <v>124092.3774577219</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.02633763317206443</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CHL</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.6955870722410734</v>
+      </c>
+      <c r="C4" t="n">
+        <v>421.964322851663</v>
+      </c>
+      <c r="D4" t="n">
+        <v>75213.85905813953</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.03746482915214577</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PER</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6419039721847954</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.341126097512947</v>
+      </c>
+      <c r="D5" t="n">
+        <v>116768.3891580127</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0623488058854041</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SUR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.6072982535445874</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4.996231459783445</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9119.974236294633</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.08283402092999219</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BRA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5996083391776642</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.483865718106943</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-304395.6066071852</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.08788451999342801</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5703876575075997</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.937424933639071</v>
+      </c>
+      <c r="D8" t="n">
+        <v>41133.41418615848</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1087766912558362</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ECU</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5523347760594717</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6.214116157655649</v>
+      </c>
+      <c r="D9" t="n">
+        <v>15063.92295309163</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1230531024244793</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>VEN</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.4367948232317739</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9928052043698148</v>
+      </c>
+      <c r="D10" t="n">
+        <v>37126.2516346622</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.239779237989031</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ARG</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.3513733988467822</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.438411872807653</v>
+      </c>
+      <c r="D11" t="n">
+        <v>172281.8475824944</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3538042294944216</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>URY</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1523869624050938</v>
+      </c>
+      <c r="C12" t="n">
+        <v>67.02476141753287</v>
+      </c>
+      <c r="D12" t="n">
+        <v>17366.58302568799</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.6955047057618148</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PRY</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.3384923673147068</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-25.27065980765401</v>
+      </c>
+      <c r="D13" t="n">
+        <v>292937.1593391935</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.3729219732774069</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>